<commit_message>
Initial implementation for the Temperature / Weather clock Major styleguide changes
</commit_message>
<xml_diff>
--- a/design/led_mapping.xlsx
+++ b/design/led_mapping.xlsx
@@ -138,7 +138,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -161,6 +161,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -179,8 +195,106 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -188,7 +302,105 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="99">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -466,14 +678,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9:T9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="2" max="12" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.33203125" customWidth="1"/>
-    <col min="14" max="24" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="24" width="4.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:26" x14ac:dyDescent="0.2">
@@ -2623,5 +2839,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>